<commit_message>
Finished the rest of the program. Now I gotta write my report :(
</commit_message>
<xml_diff>
--- a/Verification.xlsx
+++ b/Verification.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dotsc_56\workspace\MapReduceWordCount\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Users\Ruben\workspace\MapReduceWordCount\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,18 +24,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Avg</t>
   </si>
   <si>
     <t>SUM</t>
   </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -160,6 +166,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -195,6 +218,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -350,7 +390,7 @@
   <dimension ref="A1:L100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,6 +484,13 @@
         <f t="shared" si="0"/>
         <v>53.589999999999996</v>
       </c>
+      <c r="J3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <f>MIN(H1:H11)</f>
+        <v>22.806999999999999</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -467,6 +514,13 @@
       <c r="H4">
         <f t="shared" si="0"/>
         <v>22.806999999999999</v>
+      </c>
+      <c r="J4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <f>MAX(H1:H11)</f>
+        <v>70.475999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>